<commit_message>
termodynamik schematic og pcb
</commit_message>
<xml_diff>
--- a/Måling af termodynamisk data/regnemaskine til R3 udfra ønsket effekt.xlsx
+++ b/Måling af termodynamisk data/regnemaskine til R3 udfra ønsket effekt.xlsx
@@ -395,11 +395,11 @@
     </row>
     <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="n">
         <f aca="false">A3/C3</f>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>20</v>
@@ -409,7 +409,7 @@
       </c>
       <c r="E3" s="2" t="n">
         <f aca="false">((D3*G3)-F3*B3)/(F3*B3)</f>
-        <v>29999</v>
+        <v>59999</v>
       </c>
       <c r="F3" s="2" t="n">
         <v>0.1</v>
@@ -419,7 +419,7 @@
       </c>
       <c r="H3" s="3" t="n">
         <f aca="false">G3*D3/(D3+E3)</f>
-        <v>0.049506584375722</v>
+        <v>0.0248760344284317</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
DXF til differens forstærker og komperator
</commit_message>
<xml_diff>
--- a/Måling af termodynamisk data/regnemaskine til R3 udfra ønsket effekt.xlsx
+++ b/Måling af termodynamisk data/regnemaskine til R3 udfra ønsket effekt.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t xml:space="preserve">Effekt</t>
   </si>
@@ -143,24 +143,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,75 +357,134 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I3"/>
+  <dimension ref="A2:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="9.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.89"/>
   </cols>
   <sheetData>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <f aca="false">A3/C3</f>
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>300</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <f aca="false">((D3*G3)-F3*B3)/(F3*B3)</f>
+        <v>29999</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <f aca="false">A3/C3</f>
-        <v>0.25</v>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="H3" s="4" t="n">
+        <f aca="false">G3*D3/(D3+E3)</f>
+        <v>0.049506584375722</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="B6" s="3" t="n">
+        <f aca="false">A6/C6</f>
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3" t="n">
         <v>300</v>
       </c>
-      <c r="E3" s="2" t="n">
-        <f aca="false">((D3*G3)-F3*B3)/(F3*B3)</f>
-        <v>59999</v>
-      </c>
-      <c r="F3" s="2" t="n">
+      <c r="E6" s="3" t="n">
+        <f aca="false">((D6*G6)-F6*B6)/(F6*B6)</f>
+        <v>14999</v>
+      </c>
+      <c r="F6" s="3" t="n">
         <v>0.1</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="H3" s="3" t="n">
-        <f aca="false">G3*D3/(D3+E3)</f>
-        <v>0.0248760344284317</v>
-      </c>
-      <c r="I3" s="4" t="s">
+      <c r="H6" s="4" t="n">
+        <f aca="false">G6*D6/(D6+E6)</f>
+        <v>0.0980456238969867</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>